<commit_message>
fix check add well
</commit_message>
<xml_diff>
--- a/public/files/test/report.xlsx
+++ b/public/files/test/report.xlsx
@@ -19,10 +19,10 @@
     <t>Расход электроэнергии за</t>
   </si>
   <si>
-    <t>ноябрь</t>
-  </si>
-  <si>
-    <t>Месяц 2021 года</t>
+    <t>январь</t>
+  </si>
+  <si>
+    <t>Месяц 2022 года</t>
   </si>
   <si>
     <t>Тип БУ, зав.№</t>
@@ -76,10 +76,10 @@
     <t>бурение</t>
   </si>
   <si>
-    <t>31.10.2021 19:00</t>
-  </si>
-  <si>
-    <t>01.12.2021 19:00</t>
+    <t>31.12.2021 19:00</t>
+  </si>
+  <si>
+    <t>07.02.2022 19:00</t>
   </si>
   <si>
     <t>Итого по скважине</t>
@@ -1206,96 +1206,98 @@
         <v>20</v>
       </c>
       <c r="E11" s="35">
-        <v>26658.719999999998</v>
+        <v>10509.839999999998</v>
       </c>
       <c r="F11" s="35">
-        <v>27347.040000000005</v>
+        <v>11485.44</v>
       </c>
       <c r="G11" s="35">
-        <v>14628.96</v>
+        <v>10653.839999999998</v>
       </c>
       <c r="H11" s="35">
-        <v>15862.32</v>
+        <v>23938.56</v>
       </c>
       <c r="I11" s="35">
-        <v>28027.44</v>
+        <v>26178.479999999992</v>
       </c>
       <c r="J11" s="35">
-        <v>18926.64</v>
+        <v>29482.559999999998</v>
       </c>
       <c r="K11" s="35">
-        <v>20826.720000000005</v>
+        <v>15465.599999999999</v>
       </c>
       <c r="L11" s="35">
-        <v>23473.44000000001</v>
+        <v>8470.800000000001</v>
       </c>
       <c r="M11" s="35">
-        <v>8396.639999999998</v>
+        <v>7762.32</v>
       </c>
       <c r="N11" s="35">
-        <v>17724.960000000003</v>
+        <v>9088.560000000001</v>
       </c>
       <c r="O11" s="35">
-        <v>14430.240000000003</v>
+        <v>17064.719999999998</v>
       </c>
       <c r="P11" s="35">
-        <v>8040.96</v>
+        <v>16463.519999999997</v>
       </c>
       <c r="Q11" s="35">
-        <v>7691.04</v>
+        <v>19965.6</v>
       </c>
       <c r="R11" s="35">
-        <v>7649.999999999999</v>
+        <v>21417.840000000004</v>
       </c>
       <c r="S11" s="35">
-        <v>3438.0000000000005</v>
+        <v>17626.319999999996</v>
       </c>
       <c r="T11" s="35">
-        <v>8585.28</v>
+        <v>9738</v>
       </c>
       <c r="U11" s="35">
-        <v>29568.96</v>
+        <v>11371.68</v>
       </c>
       <c r="V11" s="35">
-        <v>20001.6</v>
+        <v>10551.600000000002</v>
       </c>
       <c r="W11" s="35">
-        <v>8913.6</v>
+        <v>8655.12</v>
       </c>
       <c r="X11" s="35">
-        <v>7730.640000000001</v>
+        <v>8474.399999999998</v>
       </c>
       <c r="Y11" s="35">
-        <v>21440.16</v>
+        <v>7521.119999999999</v>
       </c>
       <c r="Z11" s="35">
-        <v>19270.08</v>
+        <v>32140.080000000005</v>
       </c>
       <c r="AA11" s="35">
-        <v>29540.16</v>
+        <v>10396.800000000001</v>
       </c>
       <c r="AB11" s="35">
-        <v>27754.559999999998</v>
+        <v>8688.240000000002</v>
       </c>
       <c r="AC11" s="35">
-        <v>13806.72</v>
+        <v>24072.479999999992</v>
       </c>
       <c r="AD11" s="35">
-        <v>33446.88000000001</v>
+        <v>30810.24000000001</v>
       </c>
       <c r="AE11" s="35">
-        <v>12577.68</v>
+        <v>23374.079999999998</v>
       </c>
       <c r="AF11" s="35">
-        <v>8521.92</v>
+        <v>13427.280000000002</v>
       </c>
       <c r="AG11" s="36">
-        <v>12070.08</v>
+        <v>10779.12</v>
       </c>
       <c r="AH11" s="35">
-        <v>9990</v>
-      </c>
-      <c r="AI11" s="37"/>
+        <v>9489.6</v>
+      </c>
+      <c r="AI11" s="37">
+        <v>2134.08</v>
+      </c>
       <c r="AJ11" s="30">
         <f>SUM(E11:AI11)</f>
       </c>

</xml_diff>